<commit_message>
Tweede fase: advies aanvragen toegevoegd
Views, logica en algoritme toegevoegd om op basis van een vragenlijst geschikte producten te vinden die aan de eisen van de klant voldoen.

Nog geen view aangemaakt voor na 'vindProducten' in adviescontroller.

TODO:
Advies aanmaken en deze returnen naar een view met overzicht
</commit_message>
<xml_diff>
--- a/Wekelijkse Planning.xlsx
+++ b/Wekelijkse Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazzy\source\repos\AOM_GIT\Adviesopmaat.nl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94313713-89A9-4DFD-9E7D-45B19F54CE97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5997DD2-F161-4736-964D-59077366324E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744CDB25-7003-4DF1-87BA-0DA2807A4D35}"/>
   </bookViews>
@@ -592,7 +592,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
   <si>
     <t>Taak</t>
   </si>
@@ -898,9 +898,6 @@
     <t>Triggerfunctie bedenken</t>
   </si>
   <si>
-    <t>Algoritmiek opdracht</t>
-  </si>
-  <si>
     <t>Documentatie</t>
   </si>
   <si>
@@ -950,6 +947,24 @@
   </si>
   <si>
     <t>SQL-trigger bedenken</t>
+  </si>
+  <si>
+    <t>Documentatie bijwerken</t>
+  </si>
+  <si>
+    <t>Afmaken taken weekend</t>
+  </si>
+  <si>
+    <t>Algoritmiek beschrijven</t>
+  </si>
+  <si>
+    <t>Code smells</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Reflecties toevoegen (3 stuks)</t>
   </si>
 </sst>
 </file>
@@ -1886,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5C946E-75C2-4CD3-A76F-3D84D954DC11}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1947,10 +1962,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>101</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>23</v>
@@ -1979,7 +1994,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="65"/>
       <c r="D5" s="21"/>
@@ -1990,96 +2005,83 @@
         <v>17</v>
       </c>
       <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="66" t="s">
+      <c r="A6" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="65" t="s">
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21" t="s">
+      <c r="B8" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="66"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
-        <v>17</v>
-      </c>
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:10">
@@ -2174,105 +2176,98 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>103</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="I19" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="66"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="22" t="s">
+      <c r="I20" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="22"/>
       <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="65"/>
-      <c r="D21" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="H21" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="66"/>
-      <c r="D22" s="22" t="s">
-        <v>17</v>
-      </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="I22" s="22"/>
       <c r="J22" s="34"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="65"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="I23" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="66"/>
-      <c r="D24" s="22" t="s">
-        <v>17</v>
-      </c>
+      <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
@@ -2283,24 +2278,26 @@
       <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="65" t="s">
-        <v>102</v>
+      <c r="A25" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>101</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="H25" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="25"/>
-      <c r="B26" s="67"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="67"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -2382,11 +2379,17 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="23"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>101</v>
+      </c>
       <c r="C33" s="65"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="E33" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
@@ -2394,11 +2397,16 @@
       <c r="J33" s="21"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="24"/>
-      <c r="B34" s="66"/>
+      <c r="A34" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>101</v>
+      </c>
       <c r="C34" s="66"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
+      <c r="E34" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
@@ -2406,10 +2414,16 @@
       <c r="J34" s="34"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="23"/>
-      <c r="B35" s="65"/>
+      <c r="A35" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>101</v>
+      </c>
       <c r="C35" s="65"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -2418,10 +2432,16 @@
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="24"/>
-      <c r="B36" s="66"/>
+      <c r="A36" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="66" t="s">
+        <v>101</v>
+      </c>
       <c r="C36" s="66"/>
-      <c r="D36" s="22"/>
+      <c r="D36" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -2430,10 +2450,16 @@
       <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="23"/>
-      <c r="B37" s="65"/>
+      <c r="A37" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>101</v>
+      </c>
       <c r="C37" s="65"/>
-      <c r="D37" s="21"/>
+      <c r="D37" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
@@ -2442,11 +2468,17 @@
       <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="24"/>
-      <c r="B38" s="66"/>
+      <c r="A38" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="66" t="s">
+        <v>101</v>
+      </c>
       <c r="C38" s="66"/>
       <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
+      <c r="E38" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
@@ -2502,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A5280D-708A-4996-975B-5F380C4ADF03}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2789,7 +2821,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="43"/>
@@ -2798,7 +2830,7 @@
     </row>
     <row r="23" spans="1:7" ht="19.5">
       <c r="A23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="11"/>
@@ -2809,7 +2841,7 @@
     </row>
     <row r="24" spans="1:7" ht="19.5">
       <c r="A24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="50" t="s">
@@ -2896,7 +2928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1658758-20E9-4BDB-A2F8-D9014FB4C4DA}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Grote update: veel functies toegevoegd
add product (incl categorieen)
edit product
delete product
kleine layout aanpassingen
communicatie tussen view en controller aangepast (viewmodel in sessie)
</commit_message>
<xml_diff>
--- a/Wekelijkse Planning.xlsx
+++ b/Wekelijkse Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazzy\source\repos\AOM_GIT\Adviesopmaat.nl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5997DD2-F161-4736-964D-59077366324E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8914D02-9872-4CDA-9478-4077B9B49AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{744CDB25-7003-4DF1-87BA-0DA2807A4D35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{744CDB25-7003-4DF1-87BA-0DA2807A4D35}"/>
   </bookViews>
   <sheets>
     <sheet name="Wekelijkse planning" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
   <si>
     <t>Taak</t>
   </si>
@@ -1901,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5C946E-75C2-4CD3-A76F-3D84D954DC11}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -2534,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A5280D-708A-4996-975B-5F380C4ADF03}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -2928,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1658758-20E9-4BDB-A2F8-D9014FB4C4DA}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3042,9 +3042,7 @@
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="B15" s="57"/>
       <c r="C15" t="s">
         <v>55</v>
       </c>

</xml_diff>